<commit_message>
Beginning collecting for ID4
</commit_message>
<xml_diff>
--- a/Documents/Schedule/Mini_Milestones.xlsx
+++ b/Documents/Schedule/Mini_Milestones.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Held a stress test for the application</t>
   </si>
   <si>
-    <t>User documentation rough draft completed</t>
-  </si>
-  <si>
     <t>ID 5 Ends</t>
   </si>
   <si>
@@ -192,6 +189,12 @@
   </si>
   <si>
     <t>Tests are implemented but still need development work to pass.</t>
+  </si>
+  <si>
+    <t>Completed on March 18</t>
+  </si>
+  <si>
+    <t>User documentation first draft completed</t>
   </si>
 </sst>
 </file>
@@ -734,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -753,10 +756,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>2</v>
@@ -770,10 +773,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -781,13 +784,13 @@
         <v>42761</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -798,10 +801,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -812,13 +815,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -829,10 +832,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -851,16 +854,16 @@
         <v>42776</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -868,16 +871,16 @@
         <v>42777</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -885,16 +888,16 @@
         <v>42779</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -902,16 +905,16 @@
         <v>42780</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -919,16 +922,16 @@
         <v>42781</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -947,16 +950,16 @@
         <v>42788</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -964,16 +967,16 @@
         <v>42792</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -981,16 +984,16 @@
         <v>42791</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -998,13 +1001,13 @@
         <v>42793</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1012,13 +1015,13 @@
         <v>42793</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1026,13 +1029,13 @@
         <v>42794</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1040,13 +1043,13 @@
         <v>42794</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1054,16 +1057,16 @@
         <v>42795</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1071,13 +1074,13 @@
         <v>42795</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1085,16 +1088,16 @@
         <v>42796</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1102,16 +1105,16 @@
         <v>42798</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1125,36 +1128,57 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>42806</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>42810</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>42811</v>
       </c>
       <c r="B28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>42811</v>
+        <v>42812</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>51</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1162,39 +1186,39 @@
         <v>42812</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
-        <v>42812</v>
+        <v>42813</v>
       </c>
       <c r="B31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
+        <v>42813</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
+        <v>42818</v>
+      </c>
+      <c r="B33" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="5">
-        <v>42813</v>
-      </c>
-      <c r="B32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="6">
-        <v>42813</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
-        <v>42818</v>
+        <v>42820</v>
       </c>
       <c r="B34" t="s">
         <v>40</v>
@@ -1202,18 +1226,18 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
-        <v>42820</v>
+        <v>42824</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
-        <v>42821</v>
+        <v>42824</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1221,7 +1245,7 @@
         <v>42824</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1229,7 +1253,7 @@
         <v>42827</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1237,7 +1261,7 @@
         <v>42831</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>

</xml_diff>